<commit_message>
Added Sound for Spectral Jump
</commit_message>
<xml_diff>
--- a/ResourceCredits.xlsx
+++ b/ResourceCredits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>Sonniss.com - GDC 2015 - Game Audio Bundle</t>
+  </si>
+  <si>
+    <t>Utilities-Mine or System activation-13</t>
+  </si>
+  <si>
+    <t>Future Weapons</t>
+  </si>
+  <si>
+    <t>SoundMorph</t>
+  </si>
+  <si>
+    <t>Start Hack, End Hack</t>
+  </si>
+  <si>
+    <t>transition t04 soft 016</t>
+  </si>
+  <si>
+    <t>Spectral Jump Skill</t>
   </si>
 </sst>
 </file>
@@ -573,7 +591,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,22 +694,50 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="6"/>
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="13">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="13">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>

</xml_diff>

<commit_message>
Added Death Sound and sound for Assassination (not implemented)
</commit_message>
<xml_diff>
--- a/ResourceCredits.xlsx
+++ b/ResourceCredits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xecli\Documents\Git\-SP3-Lone-Spectre.git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xecli\Documents\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -110,16 +110,46 @@
     <t>Start Select</t>
   </si>
   <si>
-    <t>Modular UI - Text Type-Hi Tech-003.wav</t>
-  </si>
-  <si>
-    <t>Modular UI - Data Transmissions-001</t>
-  </si>
-  <si>
     <t>Objective: Bomb Planting</t>
   </si>
   <si>
     <t>Objective: Bomb Defusing</t>
+  </si>
+  <si>
+    <t>HKAP2 Seq1.1 Hits 4</t>
+  </si>
+  <si>
+    <t>Hong Kong Action Kit - Hit Kit #2</t>
+  </si>
+  <si>
+    <t>NoizBoy</t>
+  </si>
+  <si>
+    <t>Objective: Assassination</t>
+  </si>
+  <si>
+    <t>SoundMorph - Richard Devine</t>
+  </si>
+  <si>
+    <t>Modular UI</t>
+  </si>
+  <si>
+    <t>Text Type-Hi Tech-003</t>
+  </si>
+  <si>
+    <t>Data Transmissions-001</t>
+  </si>
+  <si>
+    <t>EFX EXT .50 Cal Pistol Shots 02 A</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>Coll Anderson</t>
+  </si>
+  <si>
+    <t>Death</t>
   </si>
 </sst>
 </file>
@@ -149,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -292,11 +322,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,6 +384,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,7 +672,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +681,7 @@
     <col min="2" max="2" width="47" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="32.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="98.5703125" style="1" customWidth="1"/>
     <col min="8" max="12" width="9.140625" style="1"/>
@@ -826,16 +872,24 @@
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="7">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -846,41 +900,77 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="C9" s="7">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="7">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>

</xml_diff>

<commit_message>
Added main menu music ---- - Bug where sound engine would crash on exiting
</commit_message>
<xml_diff>
--- a/ResourceCredits.xlsx
+++ b/ResourceCredits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xecli\Documents\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xecli\Documents\Git\-SP3-Lone-Spectre.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Obtained From</t>
   </si>
   <si>
-    <t>Day 43 - 70 Days</t>
-  </si>
-  <si>
     <t>Mark Sparling</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>https://www.reddit.com/r/gamedev/comments/362c72/i_made_a_bunch_of_music_feel_free_to_use_it_in/</t>
   </si>
   <si>
-    <t>Day 16 - 70 Days</t>
-  </si>
-  <si>
     <t>Level 1</t>
   </si>
   <si>
@@ -150,6 +144,15 @@
   </si>
   <si>
     <t>Death</t>
+  </si>
+  <si>
+    <t>70 Days</t>
+  </si>
+  <si>
+    <t>Day 16</t>
+  </si>
+  <si>
+    <t>Day 55</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -715,20 +718,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7">
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="14" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>9</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
@@ -740,20 +745,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C3" s="7">
         <v>8.9583333333333334E-2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -765,22 +772,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
@@ -792,22 +799,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7">
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="G5" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
@@ -819,22 +826,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -846,22 +853,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
@@ -873,22 +880,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="7">
         <v>9.0277777777777787E-3</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
@@ -900,22 +907,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7">
         <v>9.7222222222222224E-3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -927,22 +934,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="G10" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -954,22 +961,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7">
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="G11" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>

</xml_diff>

<commit_message>
Added level 9 and some new music
</commit_message>
<xml_diff>
--- a/ResourceCredits.xlsx
+++ b/ResourceCredits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>Day 55</t>
+  </si>
+  <si>
+    <t>Day 47</t>
+  </si>
+  <si>
+    <t>Level 9</t>
+  </si>
+  <si>
+    <t>Day 48</t>
+  </si>
+  <si>
+    <t>Level 8</t>
   </si>
 </sst>
 </file>
@@ -675,7 +687,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,26 +996,54 @@
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.10347222222222223</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.11388888888888889</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>

</xml_diff>